<commit_message>
Made it so that pyruvate was also smoothed before analyzing, made small improvements
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B0F940A8-3568-40D2-8AEF-9CDAA51F2E0C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00262A6-3B25-4975-98B4-06C6711FE4DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
@@ -387,95 +387,95 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>2620.9409145253831</v>
+        <v>2609.2736383522001</v>
       </c>
       <c r="B1">
-        <v>1822.6589095819998</v>
+        <v>1805.9007177286148</v>
       </c>
       <c r="C1">
-        <v>2041.06063685955</v>
+        <v>2046.4103443698491</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2576.4147753892289</v>
+        <v>2564.0016125361822</v>
       </c>
       <c r="B2">
-        <v>1782.4684700485452</v>
+        <v>1789.1326490189319</v>
       </c>
       <c r="C2">
-        <v>1988.1611135846713</v>
+        <v>2004.2483477758676</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2782.6687082765611</v>
+        <v>2772.704339868696</v>
       </c>
       <c r="B3">
-        <v>1953.7396847588923</v>
+        <v>2115.4570036857003</v>
       </c>
       <c r="C3">
-        <v>2014.5114007388909</v>
+        <v>1982.5372340769811</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2549.5290139011231</v>
+        <v>2536.9398168969196</v>
       </c>
       <c r="B4">
-        <v>1849.3654480029363</v>
+        <v>1807.1247017933108</v>
       </c>
       <c r="C4">
-        <v>1797.9890072583194</v>
+        <v>1671.066377746281</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2894.3356695431944</v>
+        <v>2848.1774558665747</v>
       </c>
       <c r="B5">
-        <v>2410.1807943816566</v>
+        <v>2142.9881146759785</v>
       </c>
       <c r="C5">
-        <v>2221.1773007788797</v>
+        <v>2201.7820875161801</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2757.4670222721129</v>
+        <v>2669.6642882999954</v>
       </c>
       <c r="B6">
-        <v>2160.5788815594015</v>
+        <v>2312.7943745309685</v>
       </c>
       <c r="C6">
-        <v>2419.5125641699742</v>
+        <v>2382.8080603810108</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2460.0130311005914</v>
+        <v>2404.1250818237031</v>
       </c>
       <c r="B7">
-        <v>2127.2437530179341</v>
+        <v>2125.2929879211752</v>
       </c>
       <c r="C7">
-        <v>2136.61591099111</v>
+        <v>2073.5057216390678</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2584.4149557622654</v>
+        <v>2467.691911221747</v>
       </c>
       <c r="B8">
-        <v>2351.3962392733724</v>
+        <v>2069.4285611930673</v>
       </c>
       <c r="C8">
-        <v>2126.1809417510226</v>
+        <v>2059.5308696816064</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3186.0038047250755</v>
+        <v>3183.785045996166</v>
       </c>
       <c r="B9">
         <v>2098.4547370844157</v>
@@ -486,40 +486,40 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2437.9552939439918</v>
+        <v>2442.5675298805104</v>
       </c>
       <c r="B10">
-        <v>1408.4531867822791</v>
+        <v>1443.0734349368897</v>
       </c>
       <c r="C10">
-        <v>1570.299250547122</v>
+        <v>1577.4517916709854</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2286.776747872384</v>
+        <v>2285.2818322507096</v>
       </c>
       <c r="B11">
-        <v>1686.2308807702489</v>
+        <v>1678.0853514394139</v>
       </c>
       <c r="C11">
-        <v>1626.4318887989045</v>
+        <v>1621.0410838989533</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2962.7472280522934</v>
+        <v>2956.9778643979516</v>
       </c>
       <c r="B12">
-        <v>2382.0382134955166</v>
+        <v>2309.7218506473168</v>
       </c>
       <c r="C12">
-        <v>2153.5079404096796</v>
+        <v>2097.2723266668459</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3176.0181195229238</v>
+        <v>3174.1140970293991</v>
       </c>
       <c r="B13">
         <v>2482.204613906229</v>
@@ -530,7 +530,7 @@
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3191.1313194200716</v>
+        <v>3188.7019285707479</v>
       </c>
       <c r="B14">
         <v>2538.6187625932635</v>
@@ -541,7 +541,7 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3159.625807701038</v>
+        <v>3158.2049492718716</v>
       </c>
       <c r="B15">
         <v>2481.9163297845398</v>
@@ -552,7 +552,7 @@
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3059.027055412681</v>
+        <v>3056.1880566748437</v>
       </c>
       <c r="B16">
         <v>1719.0075552964661</v>

</xml_diff>

<commit_message>
After changing Fp and Fl to -Inf to +Inf, didn't help much, reverting back to previous work
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C00262A6-3B25-4975-98B4-06C6711FE4DA}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F888B8-B08D-417B-9C0F-A026F7DC02EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
@@ -387,90 +387,90 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>2609.2736383522001</v>
+        <v>2619.6710337398545</v>
       </c>
       <c r="B1">
-        <v>1805.9007177286148</v>
+        <v>1744.3261301353346</v>
       </c>
       <c r="C1">
-        <v>2046.4103443698491</v>
+        <v>1744.3746610075209</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2564.0016125361822</v>
+        <v>2422.980424162788</v>
       </c>
       <c r="B2">
-        <v>1789.1326490189319</v>
+        <v>1403.7753353357568</v>
       </c>
       <c r="C2">
-        <v>2004.2483477758676</v>
+        <v>1347.2865867830023</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2772.704339868696</v>
+        <v>2827.7480600865219</v>
       </c>
       <c r="B3">
-        <v>2115.4570036857003</v>
+        <v>2266.966322519324</v>
       </c>
       <c r="C3">
-        <v>1982.5372340769811</v>
+        <v>1933.4995920571732</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2536.9398168969196</v>
+        <v>2539.7595924399211</v>
       </c>
       <c r="B4">
-        <v>1807.1247017933108</v>
+        <v>1813.7919403213787</v>
       </c>
       <c r="C4">
-        <v>1671.066377746281</v>
+        <v>1648.8017994991731</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2848.1774558665747</v>
+        <v>2844.8584118708213</v>
       </c>
       <c r="B5">
-        <v>2142.9881146759785</v>
+        <v>1976.0549125908847</v>
       </c>
       <c r="C5">
-        <v>2201.7820875161801</v>
+        <v>2168.3385675552581</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2669.6642882999954</v>
+        <v>2552.4329862565151</v>
       </c>
       <c r="B6">
-        <v>2312.7943745309685</v>
+        <v>1795.1157047345025</v>
       </c>
       <c r="C6">
-        <v>2382.8080603810108</v>
+        <v>1891.7084305962494</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2404.1250818237031</v>
+        <v>2396.6531084939179</v>
       </c>
       <c r="B7">
-        <v>2125.2929879211752</v>
+        <v>1907.6776304748842</v>
       </c>
       <c r="C7">
-        <v>2073.5057216390678</v>
+        <v>1667.4837984331457</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2467.691911221747</v>
+        <v>2988.4021092342487</v>
       </c>
       <c r="B8">
-        <v>2069.4285611930673</v>
+        <v>2463.1835649003879</v>
       </c>
       <c r="C8">
-        <v>2059.5308696816064</v>
+        <v>2321.1985563551616</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
@@ -486,35 +486,35 @@
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2442.5675298805104</v>
+        <v>2442.5594633529463</v>
       </c>
       <c r="B10">
-        <v>1443.0734349368897</v>
+        <v>1491.3792481496946</v>
       </c>
       <c r="C10">
-        <v>1577.4517916709854</v>
+        <v>1415.3482452983621</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2285.2818322507096</v>
+        <v>2285.3777130740923</v>
       </c>
       <c r="B11">
-        <v>1678.0853514394139</v>
+        <v>1678.0274308615462</v>
       </c>
       <c r="C11">
-        <v>1621.0410838989533</v>
+        <v>1620.9433178454256</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>2956.9778643979516</v>
+        <v>3107.6240713388847</v>
       </c>
       <c r="B12">
-        <v>2309.7218506473168</v>
+        <v>2479.7036053696779</v>
       </c>
       <c r="C12">
-        <v>2097.2723266668459</v>
+        <v>2361.6320543880497</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
After setting Fp and Fl lower bound to 0, got "Better" results"
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F888B8-B08D-417B-9C0F-A026F7DC02EC}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3076057E-7F2F-41FC-8242-9B1A3C644B9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>2619.6710337398545</v>
+        <v>2632.1748002241775</v>
       </c>
       <c r="B1">
-        <v>1744.3261301353346</v>
+        <v>2133.4651017085321</v>
       </c>
       <c r="C1">
-        <v>1744.3746610075209</v>
+        <v>2059.6828857739411</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2422.980424162788</v>
+        <v>2424.3275760297829</v>
       </c>
       <c r="B2">
-        <v>1403.7753353357568</v>
+        <v>1636.0682234783621</v>
       </c>
       <c r="C2">
-        <v>1347.2865867830023</v>
+        <v>1818.6760318077977</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2827.7480600865219</v>
+        <v>2891.7242165852699</v>
       </c>
       <c r="B3">
-        <v>2266.966322519324</v>
+        <v>2193.7484676388208</v>
       </c>
       <c r="C3">
-        <v>1933.4995920571732</v>
+        <v>2138.8915593313782</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2539.7595924399211</v>
+        <v>2715.7900851241898</v>
       </c>
       <c r="B4">
-        <v>1813.7919403213787</v>
+        <v>2202.8507404223883</v>
       </c>
       <c r="C4">
-        <v>1648.8017994991731</v>
+        <v>2210.8096086272531</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2844.8584118708213</v>
+        <v>2940.5293546419316</v>
       </c>
       <c r="B5">
-        <v>1976.0549125908847</v>
+        <v>2148.0221079168919</v>
       </c>
       <c r="C5">
-        <v>2168.3385675552581</v>
+        <v>2198.8077506115974</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2552.4329862565151</v>
+        <v>2785.7146696081741</v>
       </c>
       <c r="B6">
-        <v>1795.1157047345025</v>
+        <v>2303.5575870482417</v>
       </c>
       <c r="C6">
-        <v>1891.7084305962494</v>
+        <v>2387.5653411731241</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2396.6531084939179</v>
+        <v>2398.1173670810554</v>
       </c>
       <c r="B7">
-        <v>1907.6776304748842</v>
+        <v>2115.3289376251591</v>
       </c>
       <c r="C7">
-        <v>1667.4837984331457</v>
+        <v>2074.1092841307468</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2988.4021092342487</v>
+        <v>2882.0547411567204</v>
       </c>
       <c r="B8">
-        <v>2463.1835649003879</v>
+        <v>2506.259365367097</v>
       </c>
       <c r="C8">
-        <v>2321.1985563551616</v>
+        <v>2322.0381252657962</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3183.785045996166</v>
+        <v>3159.4912238408479</v>
       </c>
       <c r="B9">
-        <v>2098.4547370844157</v>
+        <v>2252.6815123713995</v>
       </c>
       <c r="C9">
-        <v>2032.8456309263427</v>
+        <v>2035.8815171824333</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2442.5594633529463</v>
+        <v>2442.5676296694178</v>
       </c>
       <c r="B10">
-        <v>1491.3792481496946</v>
+        <v>1443.4470074285916</v>
       </c>
       <c r="C10">
-        <v>1415.3482452983621</v>
+        <v>1577.8235036845329</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2285.3777130740923</v>
+        <v>2285.2918750135318</v>
       </c>
       <c r="B11">
-        <v>1678.0274308615462</v>
+        <v>1674.3145887326211</v>
       </c>
       <c r="C11">
-        <v>1620.9433178454256</v>
+        <v>1616.9537472491388</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3107.6240713388847</v>
+        <v>3074.4885462675111</v>
       </c>
       <c r="B12">
-        <v>2479.7036053696779</v>
+        <v>2504.906804466516</v>
       </c>
       <c r="C12">
-        <v>2361.6320543880497</v>
+        <v>2362.1270015854234</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3174.1140970293991</v>
+        <v>3145.5104873942182</v>
       </c>
       <c r="B13">
-        <v>2482.204613906229</v>
+        <v>2517.3901677236399</v>
       </c>
       <c r="C13">
-        <v>2257.3095767361515</v>
+        <v>2258.3211228889404</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3188.7019285707479</v>
+        <v>3159.7893414154605</v>
       </c>
       <c r="B14">
-        <v>2538.6187625932635</v>
+        <v>2565.8316250095054</v>
       </c>
       <c r="C14">
-        <v>2288.5022984824991</v>
+        <v>2289.3730088992443</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3158.2049492718716</v>
+        <v>3128.9397244237757</v>
       </c>
       <c r="B15">
-        <v>2481.9163297845398</v>
+        <v>2515.756915603733</v>
       </c>
       <c r="C15">
-        <v>2388.8584167805361</v>
+        <v>2389.3836037928622</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3056.1880566748437</v>
+        <v>3012.3636228073856</v>
       </c>
       <c r="B16">
-        <v>1719.0075552964661</v>
+        <v>2161.4222517659405</v>
       </c>
       <c r="C16">
-        <v>1829.9345956237353</v>
+        <v>1838.133979203845</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After running the boundary conditions that we optimized for ISMRM with T1Lin lower bound = 10, made analysis changes in spreadsheet
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3076057E-7F2F-41FC-8242-9B1A3C644B9A}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F689B39D-1C6F-4E42-9D37-14BF54BA02C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>2632.1748002241775</v>
+        <v>2630.1484702492698</v>
       </c>
       <c r="B1">
-        <v>2133.4651017085321</v>
+        <v>2134.1724774265472</v>
       </c>
       <c r="C1">
-        <v>2059.6828857739411</v>
+        <v>2059.154798274425</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2424.3275760297829</v>
+        <v>2423.6079349026991</v>
       </c>
       <c r="B2">
-        <v>1636.0682234783621</v>
+        <v>1406.421030295031</v>
       </c>
       <c r="C2">
-        <v>1818.6760318077977</v>
+        <v>1701.2315806727984</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2891.7242165852699</v>
+        <v>2891.7262547040496</v>
       </c>
       <c r="B3">
-        <v>2193.7484676388208</v>
+        <v>2193.7536547415039</v>
       </c>
       <c r="C3">
-        <v>2138.8915593313782</v>
+        <v>2138.887987011994</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2715.7900851241898</v>
+        <v>2715.7902273637637</v>
       </c>
       <c r="B4">
-        <v>2202.8507404223883</v>
+        <v>2202.8567011645832</v>
       </c>
       <c r="C4">
-        <v>2210.8096086272531</v>
+        <v>2210.8064768191948</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2940.5293546419316</v>
+        <v>2940.5306950164641</v>
       </c>
       <c r="B5">
-        <v>2148.0221079168919</v>
+        <v>2148.034798690579</v>
       </c>
       <c r="C5">
-        <v>2198.8077506115974</v>
+        <v>2198.8020464359815</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2785.7146696081741</v>
+        <v>2785.7168650009248</v>
       </c>
       <c r="B6">
-        <v>2303.5575870482417</v>
+        <v>2303.563896204485</v>
       </c>
       <c r="C6">
-        <v>2387.5653411731241</v>
+        <v>2387.5631075826905</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2398.1173670810554</v>
+        <v>2397.5815275200744</v>
       </c>
       <c r="B7">
-        <v>2115.3289376251591</v>
+        <v>2111.8725650676633</v>
       </c>
       <c r="C7">
-        <v>2074.1092841307468</v>
+        <v>2071.2898662971816</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2882.0547411567204</v>
+        <v>2882.0547492517726</v>
       </c>
       <c r="B8">
-        <v>2506.259365367097</v>
+        <v>2506.2593653705144</v>
       </c>
       <c r="C8">
-        <v>2322.0381252657962</v>
+        <v>2322.0381252657562</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3159.4912238408479</v>
+        <v>3159.4912255857453</v>
       </c>
       <c r="B9">
-        <v>2252.6815123713995</v>
+        <v>2252.6815124387631</v>
       </c>
       <c r="C9">
-        <v>2035.8815171824333</v>
+        <v>2035.8815171880751</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2442.5676296694178</v>
+        <v>2442.5676874809978</v>
       </c>
       <c r="B10">
-        <v>1443.4470074285916</v>
+        <v>1443.2985593610731</v>
       </c>
       <c r="C10">
-        <v>1577.8235036845329</v>
+        <v>1578.0775832209015</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2285.2918750135318</v>
+        <v>2285.2872783357448</v>
       </c>
       <c r="B11">
-        <v>1674.3145887326211</v>
+        <v>1670.3501514908894</v>
       </c>
       <c r="C11">
-        <v>1616.9537472491388</v>
+        <v>1611.6230629012018</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3074.4885462675111</v>
+        <v>3074.4885482261579</v>
       </c>
       <c r="B12">
-        <v>2504.906804466516</v>
+        <v>2504.9068044909186</v>
       </c>
       <c r="C12">
-        <v>2362.1270015854234</v>
+        <v>2362.1270015828272</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3145.5104873942182</v>
+        <v>3145.5104891155056</v>
       </c>
       <c r="B13">
-        <v>2517.3901677236399</v>
+        <v>2517.3901677265812</v>
       </c>
       <c r="C13">
-        <v>2258.3211228889404</v>
+        <v>2258.3211231646919</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3159.7893414154605</v>
+        <v>3159.7893428970565</v>
       </c>
       <c r="B14">
-        <v>2565.8316250095054</v>
+        <v>2565.8316250216185</v>
       </c>
       <c r="C14">
-        <v>2289.3730088992443</v>
+        <v>2289.3730090404611</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3128.9397244237757</v>
+        <v>3128.9397263965379</v>
       </c>
       <c r="B15">
-        <v>2515.756915603733</v>
+        <v>2515.7569156154477</v>
       </c>
       <c r="C15">
-        <v>2389.3836037928622</v>
+        <v>2389.3836037915657</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3012.3636228073856</v>
+        <v>3012.36363244525</v>
       </c>
       <c r="B16">
-        <v>2161.4222517659405</v>
+        <v>2161.4227746618949</v>
       </c>
       <c r="C16">
-        <v>1838.133979203845</v>
+        <v>1838.1326222642756</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Changing Tarrival didn't do much
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F689B39D-1C6F-4E42-9D37-14BF54BA02C3}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F99235-4D4F-4B44-9C48-31FA8D1F734C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>2630.1484702492698</v>
+        <v>2601.8684239554491</v>
       </c>
       <c r="B1">
-        <v>2134.1724774265472</v>
+        <v>2133.4903394187268</v>
       </c>
       <c r="C1">
-        <v>2059.154798274425</v>
+        <v>2059.7275084469711</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2423.6079349026991</v>
+        <v>2283.417581285787</v>
       </c>
       <c r="B2">
-        <v>1406.421030295031</v>
+        <v>1494.9049736678382</v>
       </c>
       <c r="C2">
-        <v>1701.2315806727984</v>
+        <v>1700.7225660525737</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2891.7262547040496</v>
+        <v>2875.1540281488974</v>
       </c>
       <c r="B3">
-        <v>2193.7536547415039</v>
+        <v>2193.7678485077363</v>
       </c>
       <c r="C3">
-        <v>2138.887987011994</v>
+        <v>2138.889820529434</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2715.7902273637637</v>
+        <v>2716.5390107578428</v>
       </c>
       <c r="B4">
-        <v>2202.8567011645832</v>
+        <v>2202.8785414699923</v>
       </c>
       <c r="C4">
-        <v>2210.8064768191948</v>
+        <v>2210.8070497552576</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2940.5306950164641</v>
+        <v>2921.2417263228745</v>
       </c>
       <c r="B5">
-        <v>2148.034798690579</v>
+        <v>2147.9433594646393</v>
       </c>
       <c r="C5">
-        <v>2198.8020464359815</v>
+        <v>2198.802912162032</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2785.7168650009248</v>
+        <v>2781.5017078405867</v>
       </c>
       <c r="B6">
-        <v>2303.563896204485</v>
+        <v>2303.5786862321388</v>
       </c>
       <c r="C6">
-        <v>2387.5631075826905</v>
+        <v>2387.5638409348853</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2397.5815275200744</v>
+        <v>2446.1630423940978</v>
       </c>
       <c r="B7">
-        <v>2111.8725650676633</v>
+        <v>2357.4685080142717</v>
       </c>
       <c r="C7">
-        <v>2071.2898662971816</v>
+        <v>2273.8995891981413</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2882.0547492517726</v>
+        <v>2884.6357911765899</v>
       </c>
       <c r="B8">
-        <v>2506.2593653705144</v>
+        <v>2506.2688726822835</v>
       </c>
       <c r="C8">
-        <v>2322.0381252657562</v>
+        <v>2322.0383854150141</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3159.4912255857453</v>
+        <v>3159.6791931575567</v>
       </c>
       <c r="B9">
-        <v>2252.6815124387631</v>
+        <v>2252.6717554136508</v>
       </c>
       <c r="C9">
-        <v>2035.8815171880751</v>
+        <v>2035.8814965623105</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2442.5676874809978</v>
+        <v>2442.5674573863539</v>
       </c>
       <c r="B10">
-        <v>1443.2985593610731</v>
+        <v>1443.5584288180928</v>
       </c>
       <c r="C10">
-        <v>1578.0775832209015</v>
+        <v>1577.3614355783966</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2285.2872783357448</v>
+        <v>2163.7771558412483</v>
       </c>
       <c r="B11">
-        <v>1670.3501514908894</v>
+        <v>1666.0900062610754</v>
       </c>
       <c r="C11">
-        <v>1611.6230629012018</v>
+        <v>1596.1313243617089</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3074.4885482261579</v>
+        <v>3066.1447316021095</v>
       </c>
       <c r="B12">
-        <v>2504.9068044909186</v>
+        <v>2504.8774066351243</v>
       </c>
       <c r="C12">
-        <v>2362.1270015828272</v>
+        <v>2362.1266634315061</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3145.5104891155056</v>
+        <v>3145.3317022853021</v>
       </c>
       <c r="B13">
-        <v>2517.3901677265812</v>
+        <v>2517.3950040905615</v>
       </c>
       <c r="C13">
-        <v>2258.3211231646919</v>
+        <v>2258.3215857169948</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3159.7893428970565</v>
+        <v>3159.0007489776867</v>
       </c>
       <c r="B14">
-        <v>2565.8316250216185</v>
+        <v>2565.8378342902743</v>
       </c>
       <c r="C14">
-        <v>2289.3730090404611</v>
+        <v>2289.3734640242396</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3128.9397263965379</v>
+        <v>3127.5956997100775</v>
       </c>
       <c r="B15">
-        <v>2515.7569156154477</v>
+        <v>2515.7552776066377</v>
       </c>
       <c r="C15">
-        <v>2389.3836037915657</v>
+        <v>2389.3838300551997</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3012.36363244525</v>
+        <v>3015.4375493997914</v>
       </c>
       <c r="B16">
-        <v>2161.4227746618949</v>
+        <v>2161.4677253310683</v>
       </c>
       <c r="C16">
-        <v>1838.1326222642756</v>
+        <v>1838.1350059045205</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Really good kpl trend, but kmct4 trend has been replaced by FL like in original modeling
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{63F99235-4D4F-4B44-9C48-31FA8D1F734C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9B79D45-FBAB-4FEF-94E8-9F7E0C015889}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A1">
-        <v>2601.8684239554491</v>
+        <v>2503.413669864819</v>
       </c>
       <c r="B1">
-        <v>2133.4903394187268</v>
+        <v>1825.8615987511057</v>
       </c>
       <c r="C1">
-        <v>2059.7275084469711</v>
+        <v>1805.435296458116</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A2">
-        <v>2283.417581285787</v>
+        <v>2283.7042985547573</v>
       </c>
       <c r="B2">
-        <v>1494.9049736678382</v>
+        <v>1493.8527053304535</v>
       </c>
       <c r="C2">
-        <v>1700.7225660525737</v>
+        <v>1710.1725806226718</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A3">
-        <v>2875.1540281488974</v>
+        <v>2560.4095235270556</v>
       </c>
       <c r="B3">
-        <v>2193.7678485077363</v>
+        <v>1801.9440272403326</v>
       </c>
       <c r="C3">
-        <v>2138.889820529434</v>
+        <v>1920.2388694916276</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A4">
-        <v>2716.5390107578428</v>
+        <v>2537.9421661743072</v>
       </c>
       <c r="B4">
-        <v>2202.8785414699923</v>
+        <v>1799.864344431141</v>
       </c>
       <c r="C4">
-        <v>2210.8070497552576</v>
+        <v>1646.2595615316329</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A5">
-        <v>2921.2417263228745</v>
+        <v>2681.6711769455369</v>
       </c>
       <c r="B5">
-        <v>2147.9433594646393</v>
+        <v>1745.3775111589102</v>
       </c>
       <c r="C5">
-        <v>2198.802912162032</v>
+        <v>1711.6271243643137</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2781.5017078405867</v>
+        <v>2529.4621565535494</v>
       </c>
       <c r="B6">
-        <v>2303.5786862321388</v>
+        <v>1702.2630343354697</v>
       </c>
       <c r="C6">
-        <v>2387.5638409348853</v>
+        <v>2011.3320419227862</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A7">
-        <v>2446.1630423940978</v>
+        <v>2396.4138229327441</v>
       </c>
       <c r="B7">
-        <v>2357.4685080142717</v>
+        <v>2114.9264906491089</v>
       </c>
       <c r="C7">
-        <v>2273.8995891981413</v>
+        <v>2077.3148737878214</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A8">
-        <v>2884.6357911765899</v>
+        <v>2466.5617480975629</v>
       </c>
       <c r="B8">
-        <v>2506.2688726822835</v>
+        <v>2066.6417710190935</v>
       </c>
       <c r="C8">
-        <v>2322.0383854150141</v>
+        <v>2063.6874026853902</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A9">
-        <v>3159.6791931575567</v>
+        <v>2646.5013805246285</v>
       </c>
       <c r="B9">
-        <v>2252.6717554136508</v>
+        <v>1942.8177475121645</v>
       </c>
       <c r="C9">
-        <v>2035.8814965623105</v>
+        <v>1637.0888692757562</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A10">
-        <v>2442.5674573863539</v>
+        <v>2445.758014446571</v>
       </c>
       <c r="B10">
-        <v>1443.5584288180928</v>
+        <v>1435.6782207248878</v>
       </c>
       <c r="C10">
-        <v>1577.3614355783966</v>
+        <v>1576.9788510410804</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A11">
-        <v>2163.7771558412483</v>
+        <v>2163.7686519464837</v>
       </c>
       <c r="B11">
-        <v>1666.0900062610754</v>
+        <v>1676.8451866028288</v>
       </c>
       <c r="C11">
-        <v>1596.1313243617089</v>
+        <v>1606.5592030197213</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A12">
-        <v>3066.1447316021095</v>
+        <v>2859.3559346016937</v>
       </c>
       <c r="B12">
-        <v>2504.8774066351243</v>
+        <v>2218.6895762930831</v>
       </c>
       <c r="C12">
-        <v>2362.1266634315061</v>
+        <v>1916.9616095439039</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>3145.3317022853021</v>
+        <v>2574.3872249153419</v>
       </c>
       <c r="B13">
-        <v>2517.3950040905615</v>
+        <v>2072.2152191465848</v>
       </c>
       <c r="C13">
-        <v>2258.3215857169948</v>
+        <v>2070.4027135578858</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A14">
-        <v>3159.0007489776867</v>
+        <v>2609.5010456619448</v>
       </c>
       <c r="B14">
-        <v>2565.8378342902743</v>
+        <v>2265.6740662602192</v>
       </c>
       <c r="C14">
-        <v>2289.3734640242396</v>
+        <v>2132.4259061940784</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>3127.5956997100775</v>
+        <v>2575.2390392833559</v>
       </c>
       <c r="B15">
-        <v>2515.7552776066377</v>
+        <v>1954.5493876737485</v>
       </c>
       <c r="C15">
-        <v>2389.3838300551997</v>
+        <v>2192.9488406502014</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A16">
-        <v>3015.4375493997914</v>
+        <v>2591.9502308411556</v>
       </c>
       <c r="B16">
-        <v>2161.4677253310683</v>
+        <v>1797.3965370695403</v>
       </c>
       <c r="C16">
-        <v>1838.1350059045205</v>
+        <v>1572.5026384786988</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
This is the same data but with rmse tracked
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4311155A-76F1-4CC8-813B-9FFA60DFA021}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{70F6F638-E809-4F28-9554-EE38D496D605}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1152" yWindow="1152" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
+    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>

</xml_diff>

<commit_message>
Increasing number of iterations and function evals didn't really help at all
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{348F2F6C-3AB5-40C9-8F4C-E13668747057}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C63B0A46-08F4-4FEC-908A-E8FA41FC8133}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
@@ -442,13 +442,13 @@
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A6">
-        <v>2529.4621565535494</v>
+        <v>2528.0943407812315</v>
       </c>
       <c r="B6">
-        <v>1702.2630343354697</v>
+        <v>1703.9402562987252</v>
       </c>
       <c r="C6">
-        <v>2011.3320419227862</v>
+        <v>2002.6567533848233</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.3">
@@ -519,13 +519,13 @@
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A13">
-        <v>2574.3872249153419</v>
+        <v>2573.4628886183677</v>
       </c>
       <c r="B13">
-        <v>2072.2152191465848</v>
+        <v>2070.9124728367906</v>
       </c>
       <c r="C13">
-        <v>2070.4027135578858</v>
+        <v>2069.8969628752407</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.3">
@@ -541,13 +541,13 @@
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.3">
       <c r="A15">
-        <v>2575.2390392833559</v>
+        <v>2574.2940135886543</v>
       </c>
       <c r="B15">
-        <v>1954.5493876737485</v>
+        <v>1946.9692383072338</v>
       </c>
       <c r="C15">
-        <v>2192.9488406502014</v>
+        <v>2186.1572205028783</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
These are generated files after changing boundary condition
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{39C9A135-3C9D-4A6C-A835-CB75A23CB686}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23264BAC-E46E-4C64-82BF-CD373A4A9059}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2688" yWindow="2688" windowWidth="17280" windowHeight="8964" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
+    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -383,182 +383,182 @@
       <selection sqref="A1:C16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2503.413669864819</v>
+        <v>2503.4129649087135</v>
       </c>
       <c r="B1">
-        <v>1825.8615987511057</v>
+        <v>1836.6174073036473</v>
       </c>
       <c r="C1">
-        <v>1805.435296458116</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1818.050812614732</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2283.7042985547573</v>
+        <v>2283.7034578987145</v>
       </c>
       <c r="B2">
-        <v>1493.8527053304535</v>
+        <v>1500.5236040859768</v>
       </c>
       <c r="C2">
-        <v>1710.1725806226718</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1713.3126207235091</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2560.4095235270556</v>
+        <v>2560.152091236956</v>
       </c>
       <c r="B3">
-        <v>1801.9440272403326</v>
+        <v>1800.3479258919385</v>
       </c>
       <c r="C3">
-        <v>1920.2388694916276</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1920.5342338204127</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2537.9421661743072</v>
+        <v>2537.9419460845415</v>
       </c>
       <c r="B4">
-        <v>1799.864344431141</v>
+        <v>1799.0318743020503</v>
       </c>
       <c r="C4">
-        <v>1646.2595615316329</v>
-      </c>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1638.4285917018726</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2681.6711769455369</v>
+        <v>2681.6693380571514</v>
       </c>
       <c r="B5">
-        <v>1745.3775111589102</v>
+        <v>1744.9401510683956</v>
       </c>
       <c r="C5">
-        <v>1711.6271243643137</v>
-      </c>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1707.7516198242702</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2528.0943407812315</v>
+        <v>2528.0652230370224</v>
       </c>
       <c r="B6">
-        <v>1703.9402562987252</v>
+        <v>1707.4757882748322</v>
       </c>
       <c r="C6">
-        <v>2002.6567533848233</v>
-      </c>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2003.1236656251572</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2396.4138229327441</v>
+        <v>2396.4145100733499</v>
       </c>
       <c r="B7">
-        <v>2114.9264906491089</v>
+        <v>2114.840887107051</v>
       </c>
       <c r="C7">
-        <v>2077.3148737878214</v>
-      </c>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2076.4145363599118</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2466.5617480975629</v>
+        <v>2466.5665169556682</v>
       </c>
       <c r="B8">
-        <v>2066.6417710190935</v>
+        <v>2074.1996585625466</v>
       </c>
       <c r="C8">
-        <v>2063.6874026853902</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2070.9993408703685</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2646.5013805246285</v>
+        <v>2646.4933228697419</v>
       </c>
       <c r="B9">
-        <v>1942.8177475121645</v>
+        <v>1942.9919409553129</v>
       </c>
       <c r="C9">
-        <v>1637.0888692757562</v>
-      </c>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1637.3576506534309</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2445.758014446571</v>
+        <v>2445.7574951344163</v>
       </c>
       <c r="B10">
-        <v>1435.6782207248878</v>
+        <v>1437.5708577075886</v>
       </c>
       <c r="C10">
-        <v>1576.9788510410804</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1584.7220636104068</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2163.7686519464837</v>
+        <v>2163.7661506121285</v>
       </c>
       <c r="B11">
-        <v>1676.8451866028288</v>
+        <v>1672.0183886859197</v>
       </c>
       <c r="C11">
-        <v>1606.5592030197213</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1602.2163373852031</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2859.3559346016937</v>
+        <v>2859.3300321679417</v>
       </c>
       <c r="B12">
-        <v>2218.6895762930831</v>
+        <v>2220.3401154197459</v>
       </c>
       <c r="C12">
-        <v>1916.9616095439039</v>
-      </c>
-    </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
+        <v>1930.1062011589634</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2573.4628886183677</v>
+        <v>2573.4500117771727</v>
       </c>
       <c r="B13">
-        <v>2070.9124728367906</v>
+        <v>2069.4587285737271</v>
       </c>
       <c r="C13">
-        <v>2069.8969628752407</v>
-      </c>
-    </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2070.9582771484247</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2609.5010456619448</v>
+        <v>2609.3935857794863</v>
       </c>
       <c r="B14">
-        <v>2265.6740662602192</v>
+        <v>2264.4745278119372</v>
       </c>
       <c r="C14">
-        <v>2132.4259061940784</v>
-      </c>
-    </row>
-    <row r="15" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2131.8727646395555</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2574.2940135886543</v>
+        <v>2574.253237504885</v>
       </c>
       <c r="B15">
-        <v>1946.9692383072338</v>
+        <v>1943.0136835459234</v>
       </c>
       <c r="C15">
-        <v>2186.1572205028783</v>
-      </c>
-    </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.3">
+        <v>2182.3893458170587</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2591.9502308411556</v>
+        <v>2591.9527981864389</v>
       </c>
       <c r="B16">
-        <v>1797.3965370695403</v>
+        <v>1796.809889737392</v>
       </c>
       <c r="C16">
-        <v>1572.5026384786988</v>
+        <v>1568.4260851246033</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
After fixing that radian blunder, have negative IF, fixing now
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{23264BAC-E46E-4C64-82BF-CD373A4A9059}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BA08A14C-382F-4DEE-982B-E42FAECEFE7F}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2503.4129649087135</v>
+        <v>2503.481290811585</v>
       </c>
       <c r="B1">
-        <v>1836.6174073036473</v>
+        <v>1699.8523375677767</v>
       </c>
       <c r="C1">
-        <v>1818.050812614732</v>
+        <v>1673.9643730521309</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2283.7034578987145</v>
+        <v>2277.9971094061325</v>
       </c>
       <c r="B2">
-        <v>1500.5236040859768</v>
+        <v>1501.9362601401947</v>
       </c>
       <c r="C2">
-        <v>1713.3126207235091</v>
+        <v>1402.0288730485797</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2560.152091236956</v>
+        <v>2560.1242476724956</v>
       </c>
       <c r="B3">
-        <v>1800.3479258919385</v>
+        <v>1737.303560732443</v>
       </c>
       <c r="C3">
-        <v>1920.5342338204127</v>
+        <v>1580.4586850596445</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2537.9419460845415</v>
+        <v>2494.2668094583914</v>
       </c>
       <c r="B4">
-        <v>1799.0318743020503</v>
+        <v>1876.6353147064599</v>
       </c>
       <c r="C4">
-        <v>1638.4285917018726</v>
+        <v>1893.508775158972</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2681.6693380571514</v>
+        <v>2681.663715749919</v>
       </c>
       <c r="B5">
-        <v>1744.9401510683956</v>
+        <v>1754.5415264857279</v>
       </c>
       <c r="C5">
-        <v>1707.7516198242702</v>
+        <v>1661.4949790064081</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2528.0652230370224</v>
+        <v>2478.7615939391708</v>
       </c>
       <c r="B6">
-        <v>1707.4757882748322</v>
+        <v>1810.0447733893373</v>
       </c>
       <c r="C6">
-        <v>2003.1236656251572</v>
+        <v>1876.8746931705411</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2396.4145100733499</v>
+        <v>2396.3740662144251</v>
       </c>
       <c r="B7">
-        <v>2114.840887107051</v>
+        <v>1851.2021005594868</v>
       </c>
       <c r="C7">
-        <v>2076.4145363599118</v>
+        <v>1664.0425653320099</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2466.5665169556682</v>
+        <v>2466.9899163351297</v>
       </c>
       <c r="B8">
-        <v>2074.1996585625466</v>
+        <v>1937.8683342009456</v>
       </c>
       <c r="C8">
-        <v>2070.9993408703685</v>
+        <v>1847.6799461779342</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2646.4933228697419</v>
+        <v>2643.8902174177633</v>
       </c>
       <c r="B9">
-        <v>1942.9919409553129</v>
+        <v>1944.4321728919576</v>
       </c>
       <c r="C9">
-        <v>1637.3576506534309</v>
+        <v>1636.5747422631507</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2445.7574951344163</v>
+        <v>2394.9207777787101</v>
       </c>
       <c r="B10">
-        <v>1437.5708577075886</v>
+        <v>1496.7314448948889</v>
       </c>
       <c r="C10">
-        <v>1584.7220636104068</v>
+        <v>1449.4932515435044</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2163.7661506121285</v>
+        <v>2163.7693144377299</v>
       </c>
       <c r="B11">
-        <v>1672.0183886859197</v>
+        <v>1575.0359845990301</v>
       </c>
       <c r="C11">
-        <v>1602.2163373852031</v>
+        <v>1427.7475679716438</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2859.3300321679417</v>
+        <v>2859.2191420186659</v>
       </c>
       <c r="B12">
-        <v>2220.3401154197459</v>
+        <v>2218.1049445540334</v>
       </c>
       <c r="C12">
-        <v>1930.1062011589634</v>
+        <v>1914.8994363674237</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2573.4500117771727</v>
+        <v>2528.1905879101214</v>
       </c>
       <c r="B13">
-        <v>2069.4587285737271</v>
+        <v>1932.435834573078</v>
       </c>
       <c r="C13">
-        <v>2070.9582771484247</v>
+        <v>1794.9433085700407</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2609.3935857794863</v>
+        <v>2610.7289789880551</v>
       </c>
       <c r="B14">
-        <v>2264.4745278119372</v>
+        <v>2074.3284564691662</v>
       </c>
       <c r="C14">
-        <v>2131.8727646395555</v>
+        <v>2050.6666685628061</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2574.253237504885</v>
+        <v>2531.3176201022948</v>
       </c>
       <c r="B15">
-        <v>1943.0136835459234</v>
+        <v>1976.9826572008753</v>
       </c>
       <c r="C15">
-        <v>2182.3893458170587</v>
+        <v>1827.4805076693092</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2591.9527981864389</v>
+        <v>2592.6392331263787</v>
       </c>
       <c r="B16">
-        <v>1796.809889737392</v>
+        <v>1797.0722032246758</v>
       </c>
       <c r="C16">
-        <v>1568.4260851246033</v>
+        <v>1550.1668649135759</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Managed to get the boundary condition for Rinj working
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8DFD0DBE-9C13-49A3-9D00-B2C33FE70184}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FCF2F6-958F-4708-9D08-84E4417F62D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2340" yWindow="2340" windowWidth="21600" windowHeight="11385" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
+    <workbookView xWindow="-21516" yWindow="1152" windowWidth="21600" windowHeight="11328" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2503.481290811585</v>
+        <v>2504.3643659222066</v>
       </c>
       <c r="B1">
-        <v>1699.8523375677767</v>
+        <v>1661.9251245798198</v>
       </c>
       <c r="C1">
-        <v>1673.9643730521309</v>
+        <v>1646.5851732613664</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2277.9971094061325</v>
+        <v>2270.1765981343892</v>
       </c>
       <c r="B2">
-        <v>1501.9362601401947</v>
+        <v>1579.8198104143721</v>
       </c>
       <c r="C2">
-        <v>1402.0288730485797</v>
+        <v>1489.133339545851</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2560.1242476724956</v>
+        <v>2562.8810069624815</v>
       </c>
       <c r="B3">
-        <v>1737.303560732443</v>
+        <v>1730.2687525610861</v>
       </c>
       <c r="C3">
-        <v>1580.4586850596445</v>
+        <v>1581.0506561184002</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2494.2668094583914</v>
+        <v>2494.283679208394</v>
       </c>
       <c r="B4">
-        <v>1876.6353147064599</v>
+        <v>1874.7448644803062</v>
       </c>
       <c r="C4">
-        <v>1893.508775158972</v>
+        <v>1887.29228583497</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2681.663715749919</v>
+        <v>2689.7593451447096</v>
       </c>
       <c r="B5">
-        <v>1754.5415264857279</v>
+        <v>1755.0975951550595</v>
       </c>
       <c r="C5">
-        <v>1661.4949790064081</v>
+        <v>1693.0873374066441</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2478.7615939391708</v>
+        <v>2478.7607831112336</v>
       </c>
       <c r="B6">
-        <v>1810.0447733893373</v>
+        <v>1810.1830437242672</v>
       </c>
       <c r="C6">
-        <v>1876.8746931705411</v>
+        <v>1877.1317007992568</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2396.3740662144251</v>
+        <v>2397.2088824637735</v>
       </c>
       <c r="B7">
-        <v>1851.2021005594868</v>
+        <v>1847.2459982300322</v>
       </c>
       <c r="C7">
-        <v>1664.0425653320099</v>
+        <v>1661.2757459849156</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2466.9899163351297</v>
+        <v>2467.9969983094284</v>
       </c>
       <c r="B8">
-        <v>1937.8683342009456</v>
+        <v>1930.0313340409593</v>
       </c>
       <c r="C8">
-        <v>1847.6799461779342</v>
+        <v>1785.2178304670479</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2643.8902174177633</v>
+        <v>2643.8788032222651</v>
       </c>
       <c r="B9">
-        <v>1944.4321728919576</v>
+        <v>1943.5009763779306</v>
       </c>
       <c r="C9">
-        <v>1636.5747422631507</v>
+        <v>1635.5503062445323</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2394.9207777787101</v>
+        <v>2394.9729326343991</v>
       </c>
       <c r="B10">
-        <v>1496.7314448948889</v>
+        <v>1505.7671213936892</v>
       </c>
       <c r="C10">
-        <v>1449.4932515435044</v>
+        <v>1488.8336686548521</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2163.7693144377299</v>
+        <v>2165.3642525000978</v>
       </c>
       <c r="B11">
-        <v>1575.0359845990301</v>
+        <v>1568.9743546101593</v>
       </c>
       <c r="C11">
-        <v>1427.7475679716438</v>
+        <v>1419.0680867570668</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2859.2191420186659</v>
+        <v>2864.4907222280667</v>
       </c>
       <c r="B12">
-        <v>2218.1049445540334</v>
+        <v>2225.4880847403456</v>
       </c>
       <c r="C12">
-        <v>1914.8994363674237</v>
+        <v>1936.9306010450307</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2528.1905879101214</v>
+        <v>2528.1335510759864</v>
       </c>
       <c r="B13">
-        <v>1932.435834573078</v>
+        <v>1931.1250729409865</v>
       </c>
       <c r="C13">
-        <v>1794.9433085700407</v>
+        <v>1747.3103767153727</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2610.7289789880551</v>
+        <v>2609.7077692878297</v>
       </c>
       <c r="B14">
-        <v>2074.3284564691662</v>
+        <v>2013.3383535139442</v>
       </c>
       <c r="C14">
-        <v>2050.6666685628061</v>
+        <v>1762.6716978165794</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2531.3176201022948</v>
+        <v>2531.3178653380537</v>
       </c>
       <c r="B15">
-        <v>1976.9826572008753</v>
+        <v>1976.917005535139</v>
       </c>
       <c r="C15">
-        <v>1827.4805076693092</v>
+        <v>1827.4929104745929</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2592.6392331263787</v>
+        <v>2592.3756417833501</v>
       </c>
       <c r="B16">
-        <v>1797.0722032246758</v>
+        <v>1796.2391444922016</v>
       </c>
       <c r="C16">
-        <v>1550.1668649135759</v>
+        <v>1555.1927415373646</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Optimized Tarrival and Tbolus boundary conditions
</commit_message>
<xml_diff>
--- a/AIC7parameters_hptoolbox.xlsx
+++ b/AIC7parameters_hptoolbox.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Owner\Documents\MATLAB\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A8FCF2F6-958F-4708-9D08-84E4417F62D2}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC7A8D9B-0B2B-47BC-9417-28A1AA2F1BBE}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-21516" yWindow="1152" windowWidth="21600" windowHeight="11328" xr2:uid="{B65D87CB-1A99-48CE-8154-2300C513D4BA}"/>
   </bookViews>
@@ -387,178 +387,178 @@
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1">
-        <v>2504.3643659222066</v>
+        <v>2504.364289323195</v>
       </c>
       <c r="B1">
-        <v>1661.9251245798198</v>
+        <v>1661.6143602618283</v>
       </c>
       <c r="C1">
-        <v>1646.5851732613664</v>
+        <v>1646.5366247501909</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>2270.1765981343892</v>
+        <v>2262.5421562324705</v>
       </c>
       <c r="B2">
-        <v>1579.8198104143721</v>
+        <v>1496.453505828991</v>
       </c>
       <c r="C2">
-        <v>1489.133339545851</v>
+        <v>1377.738777858284</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2562.8810069624815</v>
+        <v>2560.3680356515761</v>
       </c>
       <c r="B3">
-        <v>1730.2687525610861</v>
+        <v>1740.6496284113091</v>
       </c>
       <c r="C3">
-        <v>1581.0506561184002</v>
+        <v>1579.1624269513977</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2494.283679208394</v>
+        <v>2494.2867125411713</v>
       </c>
       <c r="B4">
-        <v>1874.7448644803062</v>
+        <v>1874.5164460460646</v>
       </c>
       <c r="C4">
-        <v>1887.29228583497</v>
+        <v>1886.2354526950858</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>2689.7593451447096</v>
+        <v>2528.8055215260533</v>
       </c>
       <c r="B5">
-        <v>1755.0975951550595</v>
+        <v>1750.1804431919084</v>
       </c>
       <c r="C5">
-        <v>1693.0873374066441</v>
+        <v>1760.0114777685721</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>2478.7607831112336</v>
+        <v>2478.757367532743</v>
       </c>
       <c r="B6">
-        <v>1810.1830437242672</v>
+        <v>1811.2349942280243</v>
       </c>
       <c r="C6">
-        <v>1877.1317007992568</v>
+        <v>1879.3514180160771</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>2397.2088824637735</v>
+        <v>2397.2088814474905</v>
       </c>
       <c r="B7">
-        <v>1847.2459982300322</v>
+        <v>1847.2451428867341</v>
       </c>
       <c r="C7">
-        <v>1661.2757459849156</v>
+        <v>1661.3136774658951</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>2467.9969983094284</v>
+        <v>2467.9969983093979</v>
       </c>
       <c r="B8">
-        <v>1930.0313340409593</v>
+        <v>1930.0311863717509</v>
       </c>
       <c r="C8">
-        <v>1785.2178304670479</v>
+        <v>1785.2194460321598</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>2643.8788032222651</v>
+        <v>2643.8794847871554</v>
       </c>
       <c r="B9">
-        <v>1943.5009763779306</v>
+        <v>1943.556967011476</v>
       </c>
       <c r="C9">
-        <v>1635.5503062445323</v>
+        <v>1635.6171814922895</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>2394.9729326343991</v>
+        <v>2394.9100585197939</v>
       </c>
       <c r="B10">
-        <v>1505.7671213936892</v>
+        <v>1487.7934969043979</v>
       </c>
       <c r="C10">
-        <v>1488.8336686548521</v>
+        <v>1468.8572344874269</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>2165.3642525000978</v>
+        <v>2163.0420362341006</v>
       </c>
       <c r="B11">
-        <v>1568.9743546101593</v>
+        <v>1575.427128416758</v>
       </c>
       <c r="C11">
-        <v>1419.0680867570668</v>
+        <v>1407.2591421929676</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>2864.4907222280667</v>
+        <v>2770.6264727355519</v>
       </c>
       <c r="B12">
-        <v>2225.4880847403456</v>
+        <v>2193.9456227505539</v>
       </c>
       <c r="C12">
-        <v>1936.9306010450307</v>
+        <v>1875.2102266616878</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>2528.1335510759864</v>
+        <v>2528.1335108469902</v>
       </c>
       <c r="B13">
-        <v>1931.1250729409865</v>
+        <v>1931.1465399730125</v>
       </c>
       <c r="C13">
-        <v>1747.3103767153727</v>
+        <v>1747.3254836145011</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>2609.7077692878297</v>
+        <v>2609.7077477574749</v>
       </c>
       <c r="B14">
-        <v>2013.3383535139442</v>
+        <v>2013.3363933907153</v>
       </c>
       <c r="C14">
-        <v>1762.6716978165794</v>
+        <v>1762.6916811467902</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>2531.3178653380537</v>
+        <v>2498.3254311829783</v>
       </c>
       <c r="B15">
-        <v>1976.917005535139</v>
+        <v>1992.2539847176738</v>
       </c>
       <c r="C15">
-        <v>1827.4929104745929</v>
+        <v>1845.4903335868835</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>2592.3756417833501</v>
+        <v>2592.375601129876</v>
       </c>
       <c r="B16">
-        <v>1796.2391444922016</v>
+        <v>1796.2307987563786</v>
       </c>
       <c r="C16">
-        <v>1555.1927415373646</v>
+        <v>1555.1632149922668</v>
       </c>
     </row>
   </sheetData>

</xml_diff>